<commit_message>
Commit 14 Wed. CS-2420 Project 2 Progress V3 start
</commit_message>
<xml_diff>
--- a/Class&Work_Schedule_V2.xlsx
+++ b/Class&Work_Schedule_V2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>   Monday   </t>
   </si>
@@ -178,13 +178,28 @@
   </si>
   <si>
     <t>9:00am</t>
+  </si>
+  <si>
+    <t>SI Office Hours</t>
+  </si>
+  <si>
+    <t>Online (30 mins)</t>
+  </si>
+  <si>
+    <t>In-person</t>
+  </si>
+  <si>
+    <t>(45 mins)</t>
+  </si>
+  <si>
+    <t>SI Planning/ Misc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,7 +289,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +383,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -454,22 +481,27 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,7 +597,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -600,7 +631,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -776,17 +806,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46:F48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -796,7 +826,7 @@
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.5">
       <c r="A1" s="17"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -814,7 +844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="22" t="s">
         <v>41</v>
       </c>
@@ -834,7 +864,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="22" t="s">
         <v>30</v>
       </c>
@@ -850,41 +880,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="15"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
+      <c r="E4" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="23"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="32" t="s">
         <v>44</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="E5" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="16"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="16"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
@@ -896,9 +932,11 @@
       </c>
       <c r="F7" s="16"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="16"/>
+    <row r="8" spans="1:6">
+      <c r="A8" s="29"/>
+      <c r="B8" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
@@ -908,9 +946,9 @@
       </c>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27" t="s">
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="29"/>
+      <c r="B9" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -922,9 +960,9 @@
       </c>
       <c r="F9" s="16"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="29"/>
+      <c r="B10" s="26" t="s">
         <v>48</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -938,9 +976,11 @@
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="18"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="29"/>
+      <c r="B11" s="33" t="s">
+        <v>58</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="3" t="s">
         <v>27</v>
@@ -948,8 +988,8 @@
       <c r="E11" s="8"/>
       <c r="F11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="29" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -958,36 +998,42 @@
       <c r="C12" s="16"/>
       <c r="D12" s="2"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="F12" s="30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="29"/>
       <c r="B13" s="4"/>
       <c r="C13" s="16"/>
       <c r="D13" s="2"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="F13" s="30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="29"/>
       <c r="B14" s="4"/>
       <c r="C14" s="16"/>
       <c r="D14" s="2"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
+      <c r="F14" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="29"/>
       <c r="B15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -996,38 +1042,38 @@
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+    <row r="17" spans="1:6">
+      <c r="A17" s="29"/>
       <c r="B17" s="2"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+    <row r="18" spans="1:6">
+      <c r="A18" s="29"/>
       <c r="B18" s="2"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="29"/>
       <c r="B19" s="2"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="29" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1046,8 +1092,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="29"/>
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
@@ -1064,8 +1110,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:6">
+      <c r="A22" s="29"/>
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1082,8 +1128,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:6">
+      <c r="A23" s="29"/>
       <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
@@ -1100,16 +1146,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:6">
+      <c r="A24" s="29"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:6">
+      <c r="A25" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="11" t="s">
@@ -1128,16 +1174,16 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:6">
+      <c r="A26" s="29"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:6">
+      <c r="A27" s="29"/>
       <c r="B27" s="16"/>
       <c r="C27" s="12" t="s">
         <v>13</v>
@@ -1148,8 +1194,8 @@
       </c>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:6">
+      <c r="A28" s="29"/>
       <c r="B28" s="16"/>
       <c r="C28" s="12" t="s">
         <v>14</v>
@@ -1160,8 +1206,8 @@
       </c>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+    <row r="29" spans="1:6">
+      <c r="A29" s="29" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="16"/>
@@ -1174,8 +1220,8 @@
       </c>
       <c r="F29" s="16"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+    <row r="30" spans="1:6">
+      <c r="A30" s="29"/>
       <c r="B30" s="16"/>
       <c r="C30" s="12" t="s">
         <v>16</v>
@@ -1186,24 +1232,24 @@
       </c>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
+    <row r="31" spans="1:6">
+      <c r="A31" s="29"/>
       <c r="B31" s="16"/>
       <c r="C31" s="13"/>
       <c r="D31" s="16"/>
       <c r="E31" s="13"/>
       <c r="F31" s="16"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="29"/>
       <c r="B32" s="16"/>
       <c r="C32" s="9"/>
       <c r="D32" s="16"/>
       <c r="E32" s="9"/>
       <c r="F32" s="16"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+    <row r="33" spans="1:6">
+      <c r="A33" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="16"/>
@@ -1216,8 +1262,8 @@
       </c>
       <c r="F33" s="16"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
+    <row r="34" spans="1:6">
+      <c r="A34" s="29"/>
       <c r="B34" s="16"/>
       <c r="C34" s="12" t="s">
         <v>18</v>
@@ -1228,8 +1274,8 @@
       </c>
       <c r="F34" s="16"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
+    <row r="35" spans="1:6">
+      <c r="A35" s="29"/>
       <c r="B35" s="16"/>
       <c r="C35" s="12" t="s">
         <v>19</v>
@@ -1240,8 +1286,8 @@
       </c>
       <c r="F35" s="16"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+    <row r="36" spans="1:6">
+      <c r="A36" s="29"/>
       <c r="B36" s="16"/>
       <c r="C36" s="12" t="s">
         <v>20</v>
@@ -1252,95 +1298,101 @@
       </c>
       <c r="F36" s="16"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="37" spans="1:6">
+      <c r="A37" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="31" t="s">
         <v>46</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="29"/>
       <c r="B38" s="16"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="32" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="16"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+    <row r="39" spans="1:6">
+      <c r="A39" s="29"/>
       <c r="B39" s="16"/>
       <c r="C39" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="33"/>
       <c r="E39" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F39" s="16"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+    <row r="40" spans="1:6">
+      <c r="A40" s="29"/>
       <c r="B40" s="16"/>
       <c r="C40" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="4"/>
+      <c r="D40" s="34"/>
       <c r="E40" s="12" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="16"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+    <row r="41" spans="1:6">
+      <c r="A41" s="29" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="16"/>
       <c r="C41" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="E41" s="12" t="s">
         <v>23</v>
       </c>
       <c r="F41" s="16"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
+    <row r="42" spans="1:6">
+      <c r="A42" s="29"/>
       <c r="B42" s="16"/>
       <c r="C42" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="16"/>
+      <c r="D42" s="30" t="s">
+        <v>56</v>
+      </c>
       <c r="E42" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F42" s="16"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
+    <row r="43" spans="1:6">
+      <c r="A43" s="29"/>
       <c r="B43" s="16"/>
       <c r="C43" s="13"/>
-      <c r="D43" s="16"/>
+      <c r="D43" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="E43" s="13"/>
       <c r="F43" s="16"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+    <row r="44" spans="1:6">
+      <c r="A44" s="29"/>
       <c r="B44" s="16"/>
       <c r="C44" s="25"/>
-      <c r="D44" s="16"/>
+      <c r="D44" s="25"/>
       <c r="E44" s="25"/>
       <c r="F44" s="16"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75">
       <c r="A45" s="24" t="s">
         <v>40</v>
       </c>
@@ -1350,37 +1402,37 @@
       <c r="C45" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="30" t="s">
+      <c r="E45" s="27" t="s">
         <v>49</v>
       </c>
       <c r="F45" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="E46" s="27" t="s">
         <v>52</v>
       </c>
       <c r="F46" s="16"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75">
       <c r="A48" s="24" t="s">
         <v>51</v>
       </c>
@@ -1396,15 +1448,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A41:A44"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" display="https://uvaps.uvu.edu/DADNormal/bwskfshd.P_CrseSchdDetl?term_in=201520&amp;crn=10917"/>
@@ -1467,24 +1519,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>